<commit_message>
finding cliques in compatibility graph.
</commit_message>
<xml_diff>
--- a/res/components/cleaned_data_xlsx/cleaned_ssd_specs_versus.xlsx
+++ b/res/components/cleaned_data_xlsx/cleaned_ssd_specs_versus.xlsx
@@ -15748,7 +15748,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K312" t="b">
@@ -16272,7 +16272,7 @@
       </c>
       <c r="J323" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K323" t="b">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="J327" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K327" t="b">
@@ -16798,7 +16798,7 @@
       </c>
       <c r="J334" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K334" t="b">
@@ -17130,7 +17130,7 @@
       </c>
       <c r="J341" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K341" t="b">
@@ -17566,7 +17566,7 @@
       <c r="I350" t="inlineStr"/>
       <c r="J350" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K350" t="b">
@@ -18050,7 +18050,7 @@
       </c>
       <c r="J360" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K360" t="b">
@@ -18094,7 +18094,7 @@
       <c r="I361" t="inlineStr"/>
       <c r="J361" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K361" t="b">
@@ -18240,7 +18240,7 @@
       </c>
       <c r="J364" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K364" t="b">
@@ -18532,7 +18532,7 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K370" t="b">
@@ -18968,7 +18968,7 @@
       </c>
       <c r="J379" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K379" t="b">
@@ -19056,7 +19056,7 @@
       <c r="I381" t="inlineStr"/>
       <c r="J381" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K381" t="b">
@@ -19584,7 +19584,7 @@
       </c>
       <c r="J392" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K392" t="b">
@@ -19824,7 +19824,7 @@
       </c>
       <c r="J397" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K397" t="b">
@@ -19870,7 +19870,7 @@
       </c>
       <c r="J398" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K398" t="b">
@@ -19968,7 +19968,7 @@
       </c>
       <c r="J400" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K400" t="b">
@@ -20016,7 +20016,7 @@
       </c>
       <c r="J401" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K401" t="b">
@@ -20206,7 +20206,7 @@
       </c>
       <c r="J405" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K405" t="b">
@@ -20254,7 +20254,7 @@
       </c>
       <c r="J406" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K406" t="b">
@@ -20346,7 +20346,7 @@
       </c>
       <c r="J408" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K408" t="b">
@@ -20390,7 +20390,7 @@
       <c r="I409" t="inlineStr"/>
       <c r="J409" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K409" t="b">
@@ -20438,7 +20438,7 @@
       </c>
       <c r="J410" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K410" t="b">
@@ -20486,7 +20486,7 @@
       </c>
       <c r="J411" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K411" t="b">
@@ -20534,7 +20534,7 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K412" t="b">
@@ -20872,7 +20872,7 @@
       </c>
       <c r="J419" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K419" t="b">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="J421" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K421" t="b">
@@ -21114,7 +21114,7 @@
       </c>
       <c r="J424" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K424" t="b">
@@ -21304,7 +21304,7 @@
       </c>
       <c r="J428" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K428" t="b">
@@ -21350,7 +21350,7 @@
       </c>
       <c r="J429" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K429" t="b">
@@ -21444,7 +21444,7 @@
       </c>
       <c r="J431" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K431" t="b">
@@ -21538,7 +21538,7 @@
       <c r="I433" t="inlineStr"/>
       <c r="J433" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K433" t="b">
@@ -21630,7 +21630,7 @@
       </c>
       <c r="J435" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K435" t="b">
@@ -21772,7 +21772,7 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K438" t="b">
@@ -21816,7 +21816,7 @@
       <c r="I439" t="inlineStr"/>
       <c r="J439" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K439" t="b">
@@ -21862,7 +21862,7 @@
       </c>
       <c r="J440" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K440" t="b">
@@ -21958,7 +21958,7 @@
       </c>
       <c r="J442" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K442" t="b">
@@ -22144,7 +22144,7 @@
       </c>
       <c r="J446" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K446" t="b">
@@ -22238,7 +22238,7 @@
       </c>
       <c r="J448" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K448" t="b">
@@ -22280,7 +22280,7 @@
       <c r="I449" t="inlineStr"/>
       <c r="J449" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K449" t="b">
@@ -22474,7 +22474,7 @@
       </c>
       <c r="J453" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K453" t="b">
@@ -22520,7 +22520,7 @@
       </c>
       <c r="J454" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K454" t="b">
@@ -22568,7 +22568,7 @@
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K455" t="b">
@@ -22616,7 +22616,7 @@
       </c>
       <c r="J456" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K456" t="b">
@@ -22660,7 +22660,7 @@
       <c r="I457" t="inlineStr"/>
       <c r="J457" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K457" t="b">
@@ -22758,7 +22758,7 @@
       </c>
       <c r="J459" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K459" t="b">
@@ -22850,7 +22850,7 @@
       </c>
       <c r="J461" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K461" t="b">
@@ -22894,7 +22894,7 @@
       <c r="I462" t="inlineStr"/>
       <c r="J462" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K462" t="b">
@@ -23136,7 +23136,7 @@
       </c>
       <c r="J467" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K467" t="b">
@@ -23230,7 +23230,7 @@
       </c>
       <c r="J469" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K469" t="b">
@@ -23278,7 +23278,7 @@
       </c>
       <c r="J470" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K470" t="b">
@@ -23326,7 +23326,7 @@
       </c>
       <c r="J471" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K471" t="b">
@@ -23374,7 +23374,7 @@
       </c>
       <c r="J472" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K472" t="b">
@@ -23420,7 +23420,7 @@
       </c>
       <c r="J473" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K473" t="b">
@@ -23468,7 +23468,7 @@
       </c>
       <c r="J474" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K474" t="b">
@@ -23516,7 +23516,7 @@
       </c>
       <c r="J475" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K475" t="b">
@@ -23564,7 +23564,7 @@
       </c>
       <c r="J476" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K476" t="b">
@@ -23612,7 +23612,7 @@
       </c>
       <c r="J477" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K477" t="b">
@@ -23660,7 +23660,7 @@
       </c>
       <c r="J478" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K478" t="b">
@@ -23754,7 +23754,7 @@
       </c>
       <c r="J480" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K480" t="b">
@@ -23802,7 +23802,7 @@
       </c>
       <c r="J481" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K481" t="b">
@@ -23946,7 +23946,7 @@
       </c>
       <c r="J484" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K484" t="b">
@@ -23994,7 +23994,7 @@
       </c>
       <c r="J485" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K485" t="b">
@@ -24042,7 +24042,7 @@
       </c>
       <c r="J486" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K486" t="b">
@@ -24088,7 +24088,7 @@
       </c>
       <c r="J487" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K487" t="b">
@@ -24136,7 +24136,7 @@
       </c>
       <c r="J488" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K488" t="b">
@@ -24184,7 +24184,7 @@
       </c>
       <c r="J489" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K489" t="b">
@@ -24330,7 +24330,7 @@
       </c>
       <c r="J492" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K492" t="b">
@@ -24378,7 +24378,7 @@
       </c>
       <c r="J493" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K493" t="b">
@@ -24472,7 +24472,7 @@
       </c>
       <c r="J495" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K495" t="b">
@@ -24520,7 +24520,7 @@
       </c>
       <c r="J496" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K496" t="b">
@@ -24568,7 +24568,7 @@
       </c>
       <c r="J497" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K497" t="b">
@@ -24662,7 +24662,7 @@
       </c>
       <c r="J499" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K499" t="b">
@@ -24710,7 +24710,7 @@
       </c>
       <c r="J500" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K500" t="b">
@@ -24758,7 +24758,7 @@
       </c>
       <c r="J501" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K501" t="b">
@@ -24850,7 +24850,7 @@
       </c>
       <c r="J503" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K503" t="b">
@@ -24896,7 +24896,7 @@
       </c>
       <c r="J504" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K504" t="b">
@@ -24944,7 +24944,7 @@
       </c>
       <c r="J505" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K505" t="b">
@@ -24992,7 +24992,7 @@
       </c>
       <c r="J506" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K506" t="b">
@@ -25126,7 +25126,7 @@
       </c>
       <c r="J509" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K509" t="b">
@@ -25172,7 +25172,7 @@
       </c>
       <c r="J510" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K510" t="b">
@@ -25214,7 +25214,7 @@
       </c>
       <c r="J511" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K511" t="b">
@@ -25260,7 +25260,7 @@
       </c>
       <c r="J512" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K512" t="b">
@@ -25308,7 +25308,7 @@
       </c>
       <c r="J513" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K513" t="b">
@@ -25356,7 +25356,7 @@
       </c>
       <c r="J514" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K514" t="b">
@@ -25446,7 +25446,7 @@
       <c r="I516" t="inlineStr"/>
       <c r="J516" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K516" t="b">
@@ -25536,7 +25536,7 @@
       </c>
       <c r="J518" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K518" t="b">
@@ -25674,7 +25674,7 @@
       </c>
       <c r="J521" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K521" t="b">
@@ -25764,7 +25764,7 @@
       <c r="I523" t="inlineStr"/>
       <c r="J523" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K523" t="b">
@@ -25810,7 +25810,7 @@
       </c>
       <c r="J524" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K524" t="b">
@@ -25858,7 +25858,7 @@
       </c>
       <c r="J525" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K525" t="b">
@@ -25952,7 +25952,7 @@
       <c r="I527" t="inlineStr"/>
       <c r="J527" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K527" t="b">
@@ -26046,7 +26046,7 @@
       </c>
       <c r="J529" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K529" t="b">
@@ -26094,7 +26094,7 @@
       </c>
       <c r="J530" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K530" t="b">
@@ -26140,7 +26140,7 @@
       </c>
       <c r="J531" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K531" t="b">
@@ -26188,7 +26188,7 @@
       </c>
       <c r="J532" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K532" t="b">
@@ -26280,7 +26280,7 @@
       </c>
       <c r="J534" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K534" t="b">
@@ -26328,7 +26328,7 @@
       </c>
       <c r="J535" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K535" t="b">
@@ -26376,7 +26376,7 @@
       </c>
       <c r="J536" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K536" t="b">
@@ -26514,7 +26514,7 @@
       </c>
       <c r="J539" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K539" t="b">
@@ -26562,7 +26562,7 @@
       </c>
       <c r="J540" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K540" t="b">
@@ -26608,7 +26608,7 @@
       </c>
       <c r="J541" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K541" t="b">
@@ -26940,7 +26940,7 @@
       </c>
       <c r="J548" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K548" t="b">
@@ -26982,7 +26982,7 @@
       <c r="I549" t="inlineStr"/>
       <c r="J549" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K549" t="b">
@@ -27026,7 +27026,7 @@
       <c r="I550" t="inlineStr"/>
       <c r="J550" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K550" t="b">
@@ -27074,7 +27074,7 @@
       </c>
       <c r="J551" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K551" t="b">
@@ -27122,7 +27122,7 @@
       </c>
       <c r="J552" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K552" t="b">
@@ -27168,7 +27168,7 @@
       </c>
       <c r="J553" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K553" t="b">
@@ -27214,7 +27214,7 @@
       </c>
       <c r="J554" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K554" t="b">
@@ -27260,7 +27260,7 @@
       </c>
       <c r="J555" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K555" t="b">
@@ -27354,7 +27354,7 @@
       </c>
       <c r="J557" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K557" t="b">
@@ -27494,7 +27494,7 @@
       </c>
       <c r="J560" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K560" t="b">
@@ -27536,7 +27536,7 @@
       <c r="I561" t="inlineStr"/>
       <c r="J561" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K561" t="b">
@@ -27580,7 +27580,7 @@
       <c r="I562" t="inlineStr"/>
       <c r="J562" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K562" t="b">
@@ -27624,7 +27624,7 @@
       <c r="I563" t="inlineStr"/>
       <c r="J563" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K563" t="b">
@@ -27672,7 +27672,7 @@
       </c>
       <c r="J564" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K564" t="b">
@@ -27720,7 +27720,7 @@
       </c>
       <c r="J565" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K565" t="b">
@@ -27766,7 +27766,7 @@
       </c>
       <c r="J566" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K566" t="b">
@@ -27812,7 +27812,7 @@
       </c>
       <c r="J567" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K567" t="b">
@@ -27854,7 +27854,7 @@
       <c r="I568" t="inlineStr"/>
       <c r="J568" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K568" t="b">
@@ -27898,7 +27898,7 @@
       <c r="I569" t="inlineStr"/>
       <c r="J569" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K569" t="b">
@@ -27946,7 +27946,7 @@
       </c>
       <c r="J570" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K570" t="b">
@@ -27990,7 +27990,7 @@
       <c r="I571" t="inlineStr"/>
       <c r="J571" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K571" t="b">
@@ -28038,7 +28038,7 @@
       </c>
       <c r="J572" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K572" t="b">
@@ -28084,7 +28084,7 @@
       </c>
       <c r="J573" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K573" t="b">
@@ -28132,7 +28132,7 @@
       </c>
       <c r="J574" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K574" t="b">
@@ -28178,7 +28178,7 @@
       </c>
       <c r="J575" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K575" t="b">
@@ -28224,7 +28224,7 @@
       </c>
       <c r="J576" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K576" t="b">
@@ -28266,7 +28266,7 @@
       <c r="I577" t="inlineStr"/>
       <c r="J577" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K577" t="b">
@@ -28310,7 +28310,7 @@
       <c r="I578" t="inlineStr"/>
       <c r="J578" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K578" t="b">
@@ -28358,7 +28358,7 @@
       </c>
       <c r="J579" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K579" t="b">
@@ -28404,7 +28404,7 @@
       </c>
       <c r="J580" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K580" t="b">
@@ -28450,7 +28450,7 @@
       </c>
       <c r="J581" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K581" t="b">
@@ -28498,7 +28498,7 @@
       </c>
       <c r="J582" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K582" t="b">
@@ -28586,7 +28586,7 @@
       <c r="I584" t="inlineStr"/>
       <c r="J584" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K584" t="b">
@@ -28634,7 +28634,7 @@
       </c>
       <c r="J585" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K585" t="b">
@@ -28676,7 +28676,7 @@
       <c r="I586" t="inlineStr"/>
       <c r="J586" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K586" t="b">
@@ -28720,7 +28720,7 @@
       <c r="I587" t="inlineStr"/>
       <c r="J587" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K587" t="b">
@@ -28764,7 +28764,7 @@
       <c r="I588" t="inlineStr"/>
       <c r="J588" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K588" t="b">
@@ -28812,7 +28812,7 @@
       </c>
       <c r="J589" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K589" t="b">
@@ -28854,7 +28854,7 @@
       <c r="I590" t="inlineStr"/>
       <c r="J590" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K590" t="b">
@@ -28902,7 +28902,7 @@
       </c>
       <c r="J591" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K591" t="b">
@@ -28944,7 +28944,7 @@
       <c r="I592" t="inlineStr"/>
       <c r="J592" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K592" t="b">
@@ -28992,7 +28992,7 @@
       </c>
       <c r="J593" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K593" t="b">
@@ -29038,7 +29038,7 @@
       </c>
       <c r="J594" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K594" t="b">
@@ -29086,7 +29086,7 @@
       </c>
       <c r="J595" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K595" t="b">
@@ -29130,7 +29130,7 @@
       </c>
       <c r="J596" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K596" t="b">
@@ -29174,7 +29174,7 @@
       <c r="I597" t="inlineStr"/>
       <c r="J597" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K597" t="b">
@@ -29218,7 +29218,7 @@
       <c r="I598" t="inlineStr"/>
       <c r="J598" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K598" t="b">
@@ -29266,7 +29266,7 @@
       </c>
       <c r="J599" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K599" t="b">
@@ -29312,7 +29312,7 @@
       </c>
       <c r="J600" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K600" t="b">
@@ -29354,7 +29354,7 @@
       <c r="I601" t="inlineStr"/>
       <c r="J601" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K601" t="b">
@@ -29398,7 +29398,7 @@
       <c r="I602" t="inlineStr"/>
       <c r="J602" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K602" t="b">
@@ -29444,7 +29444,7 @@
       </c>
       <c r="J603" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K603" t="b">
@@ -29486,7 +29486,7 @@
       <c r="I604" t="inlineStr"/>
       <c r="J604" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K604" t="b">
@@ -29528,7 +29528,7 @@
       <c r="I605" t="inlineStr"/>
       <c r="J605" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K605" t="b">
@@ -29574,7 +29574,7 @@
       </c>
       <c r="J606" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K606" t="b">
@@ -29620,7 +29620,7 @@
       </c>
       <c r="J607" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K607" t="b">
@@ -29664,7 +29664,7 @@
       <c r="I608" t="inlineStr"/>
       <c r="J608" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K608" t="b">
@@ -29712,7 +29712,7 @@
       </c>
       <c r="J609" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K609" t="b">
@@ -29756,7 +29756,7 @@
       <c r="I610" t="inlineStr"/>
       <c r="J610" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K610" t="b">
@@ -29804,7 +29804,7 @@
       </c>
       <c r="J611" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K611" t="b">
@@ -29852,7 +29852,7 @@
       </c>
       <c r="J612" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K612" t="b">
@@ -29894,7 +29894,7 @@
       <c r="I613" t="inlineStr"/>
       <c r="J613" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K613" t="b">
@@ -29938,7 +29938,7 @@
       <c r="I614" t="inlineStr"/>
       <c r="J614" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K614" t="b">
@@ -29982,7 +29982,7 @@
       <c r="I615" t="inlineStr"/>
       <c r="J615" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K615" t="b">
@@ -30030,7 +30030,7 @@
       </c>
       <c r="J616" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K616" t="b">
@@ -30078,7 +30078,7 @@
       </c>
       <c r="J617" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K617" t="b">
@@ -30126,7 +30126,7 @@
       </c>
       <c r="J618" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K618" t="b">
@@ -30170,7 +30170,7 @@
       <c r="I619" t="inlineStr"/>
       <c r="J619" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K619" t="b">
@@ -30216,7 +30216,7 @@
       </c>
       <c r="J620" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K620" t="b">
@@ -30260,7 +30260,7 @@
       <c r="I621" t="inlineStr"/>
       <c r="J621" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K621" t="b">
@@ -30308,7 +30308,7 @@
       </c>
       <c r="J622" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K622" t="b">
@@ -30356,7 +30356,7 @@
       </c>
       <c r="J623" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K623" t="b">
@@ -30404,7 +30404,7 @@
       </c>
       <c r="J624" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K624" t="b">
@@ -30446,7 +30446,7 @@
       <c r="I625" t="inlineStr"/>
       <c r="J625" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K625" t="b">
@@ -30494,7 +30494,7 @@
       </c>
       <c r="J626" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K626" t="b">
@@ -30542,7 +30542,7 @@
       </c>
       <c r="J627" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K627" t="b">
@@ -30590,7 +30590,7 @@
       </c>
       <c r="J628" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K628" t="b">
@@ -30636,7 +30636,7 @@
       </c>
       <c r="J629" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K629" t="b">
@@ -30680,7 +30680,7 @@
       <c r="I630" t="inlineStr"/>
       <c r="J630" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K630" t="b">
@@ -30726,7 +30726,7 @@
       </c>
       <c r="J631" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K631" t="b">
@@ -30774,7 +30774,7 @@
       </c>
       <c r="J632" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K632" t="b">
@@ -30822,7 +30822,7 @@
       </c>
       <c r="J633" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K633" t="b">
@@ -30868,7 +30868,7 @@
       </c>
       <c r="J634" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K634" t="b">
@@ -30914,7 +30914,7 @@
       </c>
       <c r="J635" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K635" t="b">
@@ -30958,7 +30958,7 @@
       </c>
       <c r="J636" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K636" t="b">
@@ -31006,7 +31006,7 @@
       </c>
       <c r="J637" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K637" t="b">
@@ -31050,7 +31050,7 @@
       <c r="I638" t="inlineStr"/>
       <c r="J638" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K638" t="b">
@@ -31098,7 +31098,7 @@
       </c>
       <c r="J639" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K639" t="b">
@@ -31140,7 +31140,7 @@
       <c r="I640" t="inlineStr"/>
       <c r="J640" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K640" t="b">
@@ -31188,7 +31188,7 @@
       </c>
       <c r="J641" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K641" t="b">
@@ -31230,7 +31230,7 @@
       <c r="I642" t="inlineStr"/>
       <c r="J642" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K642" t="b">
@@ -31278,7 +31278,7 @@
       </c>
       <c r="J643" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K643" t="b">
@@ -31324,7 +31324,7 @@
       </c>
       <c r="J644" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K644" t="b">
@@ -31370,7 +31370,7 @@
       </c>
       <c r="J645" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K645" t="b">
@@ -31418,7 +31418,7 @@
       </c>
       <c r="J646" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K646" t="b">
@@ -31464,7 +31464,7 @@
       </c>
       <c r="J647" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K647" t="b">
@@ -31510,7 +31510,7 @@
       </c>
       <c r="J648" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K648" t="b">
@@ -31552,7 +31552,7 @@
       <c r="I649" t="inlineStr"/>
       <c r="J649" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K649" t="b">
@@ -31600,7 +31600,7 @@
       </c>
       <c r="J650" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K650" t="b">
@@ -31646,7 +31646,7 @@
       </c>
       <c r="J651" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K651" t="b">
@@ -31692,7 +31692,7 @@
       </c>
       <c r="J652" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K652" t="b">
@@ -31738,7 +31738,7 @@
       </c>
       <c r="J653" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K653" t="b">
@@ -31782,7 +31782,7 @@
       <c r="I654" t="inlineStr"/>
       <c r="J654" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K654" t="b">
@@ -31828,7 +31828,7 @@
       </c>
       <c r="J655" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K655" t="b">
@@ -31874,7 +31874,7 @@
       </c>
       <c r="J656" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K656" t="b">
@@ -31920,7 +31920,7 @@
       </c>
       <c r="J657" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K657" t="b">
@@ -31962,7 +31962,7 @@
       <c r="I658" t="inlineStr"/>
       <c r="J658" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K658" t="b">
@@ -32010,7 +32010,7 @@
       </c>
       <c r="J659" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K659" t="b">
@@ -32056,7 +32056,7 @@
       </c>
       <c r="J660" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K660" t="b">
@@ -32104,7 +32104,7 @@
       </c>
       <c r="J661" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K661" t="b">
@@ -32152,7 +32152,7 @@
       </c>
       <c r="J662" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K662" t="b">
@@ -32194,7 +32194,7 @@
       <c r="I663" t="inlineStr"/>
       <c r="J663" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K663" t="b">
@@ -32240,7 +32240,7 @@
       </c>
       <c r="J664" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K664" t="b">
@@ -32288,7 +32288,7 @@
       </c>
       <c r="J665" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K665" t="b">
@@ -32334,7 +32334,7 @@
       </c>
       <c r="J666" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K666" t="b">
@@ -32380,7 +32380,7 @@
       </c>
       <c r="J667" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K667" t="b">
@@ -32424,7 +32424,7 @@
       </c>
       <c r="J668" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K668" t="b">
@@ -32468,7 +32468,7 @@
       </c>
       <c r="J669" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K669" t="b">
@@ -32514,7 +32514,7 @@
       </c>
       <c r="J670" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K670" t="b">
@@ -32560,7 +32560,7 @@
       </c>
       <c r="J671" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K671" t="b">
@@ -32602,7 +32602,7 @@
       <c r="I672" t="inlineStr"/>
       <c r="J672" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K672" t="b">
@@ -32648,7 +32648,7 @@
       </c>
       <c r="J673" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K673" t="b">
@@ -32694,7 +32694,7 @@
       </c>
       <c r="J674" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K674" t="b">
@@ -32740,7 +32740,7 @@
       </c>
       <c r="J675" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K675" t="b">
@@ -32786,7 +32786,7 @@
       </c>
       <c r="J676" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K676" t="b">
@@ -32830,7 +32830,7 @@
       </c>
       <c r="J677" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K677" t="b">
@@ -32876,7 +32876,7 @@
       </c>
       <c r="J678" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K678" t="b">
@@ -32922,7 +32922,7 @@
       </c>
       <c r="J679" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K679" t="b">
@@ -32968,7 +32968,7 @@
       </c>
       <c r="J680" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K680" t="b">
@@ -33010,7 +33010,7 @@
       </c>
       <c r="J681" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K681" t="b">
@@ -33056,7 +33056,7 @@
       </c>
       <c r="J682" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K682" t="b">
@@ -33100,7 +33100,7 @@
       </c>
       <c r="J683" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K683" t="b">
@@ -33146,7 +33146,7 @@
       </c>
       <c r="J684" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K684" t="b">
@@ -33188,7 +33188,7 @@
       <c r="I685" t="inlineStr"/>
       <c r="J685" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K685" t="b">
@@ -33234,7 +33234,7 @@
       </c>
       <c r="J686" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K686" t="b">
@@ -33276,7 +33276,7 @@
       <c r="I687" t="inlineStr"/>
       <c r="J687" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K687" t="b">
@@ -33322,7 +33322,7 @@
       </c>
       <c r="J688" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K688" t="b">
@@ -33364,7 +33364,7 @@
       <c r="I689" t="inlineStr"/>
       <c r="J689" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K689" t="b">
@@ -33406,7 +33406,7 @@
       <c r="I690" t="inlineStr"/>
       <c r="J690" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K690" t="b">
@@ -33452,7 +33452,7 @@
       </c>
       <c r="J691" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K691" t="b">
@@ -33500,7 +33500,7 @@
       </c>
       <c r="J692" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K692" t="b">
@@ -33546,7 +33546,7 @@
       </c>
       <c r="J693" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K693" t="b">
@@ -33590,7 +33590,7 @@
       </c>
       <c r="J694" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K694" t="b">
@@ -33636,7 +33636,7 @@
       </c>
       <c r="J695" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K695" t="b">
@@ -33682,7 +33682,7 @@
       </c>
       <c r="J696" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K696" t="b">
@@ -33728,7 +33728,7 @@
       </c>
       <c r="J697" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K697" t="b">
@@ -33774,7 +33774,7 @@
       </c>
       <c r="J698" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K698" t="b">
@@ -33820,7 +33820,7 @@
       </c>
       <c r="J699" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K699" t="b">
@@ -33866,7 +33866,7 @@
       </c>
       <c r="J700" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K700" t="b">
@@ -33914,7 +33914,7 @@
       </c>
       <c r="J701" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K701" t="b">
@@ -33960,7 +33960,7 @@
       </c>
       <c r="J702" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K702" t="b">
@@ -34006,7 +34006,7 @@
       </c>
       <c r="J703" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K703" t="b">
@@ -34052,7 +34052,7 @@
       </c>
       <c r="J704" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K704" t="b">
@@ -34098,7 +34098,7 @@
       </c>
       <c r="J705" t="inlineStr">
         <is>
-          <t>2.5"</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="K705" t="b">

</xml_diff>